<commit_message>
Update Controller and Datapath
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr updateLinks="never"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BACH KHOA\Internship\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BACH KHOA\Internship\Single-cycle  Risc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB708C6-F4CA-4163-A69F-EA4AA879B28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDC3447-A256-4804-B863-D177D9FE585A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="643" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="11295" tabRatio="643" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="2" r:id="rId1"/>
@@ -50,9 +50,9 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Hung Quang. Truong - Personal View" guid="{C61E42EC-A28A-4F34-B1F0-5B0C369C3BFF}" mergeInterval="0" personalView="1" maximized="1" xWindow="-9" yWindow="-9" windowWidth="1864" windowHeight="1218" activeSheetId="6"/>
+    <customWorkbookView name="Phong Thanh. Phan - Personal View" guid="{BBCD1273-FB62-4046-AADE-F9CEEA687EB3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="5"/>
     <customWorkbookView name="Giang Truong Le. Nguyen - Personal View" guid="{D6408F3F-69A9-4377-B307-B0A0F5ECDF86}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="3"/>
-    <customWorkbookView name="Phong Thanh. Phan - Personal View" guid="{BBCD1273-FB62-4046-AADE-F9CEEA687EB3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="5"/>
-    <customWorkbookView name="Hung Quang. Truong - Personal View" guid="{C61E42EC-A28A-4F34-B1F0-5B0C369C3BFF}" mergeInterval="0" personalView="1" maximized="1" xWindow="-9" yWindow="-9" windowWidth="1864" windowHeight="1218" activeSheetId="6"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="75">
   <si>
     <t>No.</t>
   </si>
@@ -122,9 +122,6 @@
     <t>ALU_control_tb.sv</t>
   </si>
   <si>
-    <t>Simulate and compare the value of truth table with the output of the control based on the input generated by testbench</t>
-  </si>
-  <si>
     <t>single-cycle Mips processor</t>
   </si>
   <si>
@@ -141,9 +138,6 @@
   </si>
   <si>
     <t>controller_tb.sv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Simulate and compare the value of truth table with the output of the controller based on the input generated by testbench </t>
   </si>
   <si>
     <t xml:space="preserve">Check the output value when combining 2 modules control and ALU_control </t>
@@ -284,6 +278,27 @@
   <si>
     <t>top_verification_4_tb.sv</t>
   </si>
+  <si>
+    <t>Correctness</t>
+  </si>
+  <si>
+    <t>Manh Tran-Duc</t>
+  </si>
+  <si>
+    <t>Simulate and compare the correctness of output
+transactions based on the table in section 3.1.1(In file pdf)</t>
+  </si>
+  <si>
+    <t>Simulate and compare the correctness of output
+transactions based on the table in section 3.1.2(In file pdf)</t>
+  </si>
+  <si>
+    <t>Simulate and compare the correctness of output
+transactions based on the table in section 3.1.2 and 3.1.1(In file pdf)</t>
+  </si>
+  <si>
+    <t>Implement reset for REGISTER because if no value in it the output data will be X</t>
+  </si>
 </sst>
 </file>
 
@@ -292,7 +307,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="109">
+  <fonts count="110">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -1018,6 +1033,11 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="ArialMT"/>
     </font>
   </fonts>
   <fills count="54">
@@ -1339,7 +1359,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="75">
+  <borders count="76">
     <border>
       <left/>
       <right/>
@@ -2269,6 +2289,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="586">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -3680,7 +3715,7 @@
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="101" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3763,9 +3798,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="103" fillId="51" borderId="37" xfId="457" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="103" fillId="51" borderId="37" xfId="457" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="103" fillId="0" borderId="23" xfId="86" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3911,6 +3943,13 @@
     </xf>
     <xf numFmtId="49" fontId="104" fillId="50" borderId="30" xfId="86" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="109" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="103" fillId="0" borderId="53" xfId="86" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="103" fillId="0" borderId="53" xfId="86" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="586">
@@ -4501,7 +4540,433 @@
     <cellStyle name="集計 4 2" xfId="576" xr:uid="{00000000-0005-0000-0000-000048020000}"/>
     <cellStyle name="集計 5" xfId="541" xr:uid="{00000000-0005-0000-0000-000049020000}"/>
   </cellStyles>
-  <dxfs count="88">
+  <dxfs count="136">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -5743,28 +6208,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:AS72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="5.625" style="6" customWidth="1"/>
     <col min="2" max="2" width="6" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="38.21875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="9.75" style="7" customWidth="1"/>
+    <col min="5" max="5" width="38.25" style="8" customWidth="1"/>
     <col min="6" max="6" width="10" style="8" customWidth="1"/>
-    <col min="7" max="7" width="39.88671875" style="8" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="25.21875" style="9" customWidth="1"/>
-    <col min="10" max="10" width="17.33203125" style="9" customWidth="1"/>
-    <col min="11" max="11" width="51.44140625" style="9" customWidth="1"/>
-    <col min="12" max="12" width="33.21875" style="6" customWidth="1"/>
-    <col min="13" max="16384" width="5.6640625" style="6"/>
+    <col min="7" max="7" width="39.875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="15.625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="25.25" style="9" customWidth="1"/>
+    <col min="10" max="10" width="17.375" style="9" customWidth="1"/>
+    <col min="11" max="11" width="51.5" style="9" customWidth="1"/>
+    <col min="12" max="12" width="50.25" style="6" customWidth="1"/>
+    <col min="13" max="16384" width="5.625" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:45" ht="20.399999999999999">
+    <row r="2" spans="1:45" ht="20.25">
       <c r="B2" s="3"/>
       <c r="C2" s="2"/>
       <c r="D2" s="1"/>
@@ -5819,7 +6284,7 @@
       <c r="AR4" s="5"/>
       <c r="AS4" s="5"/>
     </row>
-    <row r="5" spans="1:45" s="4" customFormat="1" ht="21">
+    <row r="5" spans="1:45" s="4" customFormat="1" ht="20.25">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="11"/>
@@ -5866,18 +6331,18 @@
       <c r="AR5" s="5"/>
       <c r="AS5" s="5"/>
     </row>
-    <row r="8" spans="1:45" ht="15.6" thickBot="1"/>
-    <row r="9" spans="1:45" ht="16.2" thickBot="1">
-      <c r="B9" s="71" t="s">
+    <row r="8" spans="1:45" ht="15.75" thickBot="1"/>
+    <row r="9" spans="1:45" ht="16.5" thickBot="1">
+      <c r="B9" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="72"/>
-      <c r="D9" s="73" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="74"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="65"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="72" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="73"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="15"/>
@@ -5898,19 +6363,19 @@
       <c r="G10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="75" t="s">
+      <c r="H10" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="I10" s="75" t="s">
+      <c r="I10" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="J10" s="67" t="s">
+      <c r="J10" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="K10" s="67" t="s">
+      <c r="K10" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="L10" s="69" t="s">
+      <c r="L10" s="68" t="s">
         <v>1</v>
       </c>
       <c r="M10" s="6"/>
@@ -5934,15 +6399,15 @@
       <c r="G11" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="76"/>
-      <c r="I11" s="76"/>
-      <c r="J11" s="68"/>
-      <c r="K11" s="68"/>
-      <c r="L11" s="70"/>
+      <c r="H11" s="75"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="69"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
     </row>
-    <row r="12" spans="1:45" s="10" customFormat="1" ht="73.8" customHeight="1" thickTop="1">
+    <row r="12" spans="1:45" s="10" customFormat="1" ht="73.900000000000006" customHeight="1" thickTop="1" thickBot="1">
       <c r="A12" s="6"/>
       <c r="B12" s="22">
         <v>1</v>
@@ -5960,24 +6425,28 @@
         <v>1</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="27"/>
-      <c r="I12" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I12" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="J12" s="29"/>
-      <c r="K12" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="L12" s="31"/>
+      <c r="J12" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="K12" s="76" t="s">
+        <v>71</v>
+      </c>
+      <c r="L12" s="76"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
     </row>
-    <row r="13" spans="1:45" s="10" customFormat="1" ht="55.2" customHeight="1">
+    <row r="13" spans="1:45" s="10" customFormat="1" ht="55.15" customHeight="1" thickBot="1">
       <c r="A13" s="6"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="33"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="32"/>
       <c r="D13" s="24">
         <v>2</v>
       </c>
@@ -5987,164 +6456,190 @@
       <c r="F13" s="24">
         <v>2</v>
       </c>
-      <c r="G13" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28" t="s">
+      <c r="G13" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I13" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="J13" s="35"/>
-      <c r="K13" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="L13" s="36"/>
+      <c r="J13" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="K13" s="76" t="s">
+        <v>72</v>
+      </c>
+      <c r="L13" s="76"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
     </row>
-    <row r="14" spans="1:45" s="10" customFormat="1" ht="55.2" customHeight="1">
+    <row r="14" spans="1:45" s="10" customFormat="1" ht="55.15" customHeight="1" thickBot="1">
       <c r="A14" s="6"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="37"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="24">
         <v>3</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F14" s="24">
         <v>3</v>
       </c>
-      <c r="G14" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28" t="s">
+      <c r="G14" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="J14" s="29"/>
-      <c r="K14" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="L14" s="31"/>
+      <c r="H14" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="K14" s="76" t="s">
+        <v>73</v>
+      </c>
+      <c r="L14" s="30"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
     </row>
-    <row r="15" spans="1:45" s="10" customFormat="1" ht="55.2" customHeight="1">
+    <row r="15" spans="1:45" s="10" customFormat="1" ht="55.15" customHeight="1">
       <c r="A15" s="6"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="38"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="37"/>
       <c r="D15" s="24">
         <v>1</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F15" s="24">
         <v>1</v>
       </c>
       <c r="G15" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="H15" s="27"/>
-      <c r="I15" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="J15" s="29"/>
-      <c r="K15" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="L15" s="31"/>
+        <v>26</v>
+      </c>
+      <c r="H15" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I15" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="J15" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="K15" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" s="30"/>
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
     </row>
     <row r="16" spans="1:45" s="10" customFormat="1" ht="66" customHeight="1">
       <c r="A16" s="6"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="39" t="s">
-        <v>19</v>
+      <c r="B16" s="31"/>
+      <c r="C16" s="38" t="s">
+        <v>18</v>
       </c>
       <c r="D16" s="24">
         <v>2</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F16" s="24">
         <v>2</v>
       </c>
-      <c r="G16" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="J16" s="35"/>
-      <c r="K16" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="L16" s="36"/>
+      <c r="G16" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I16" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="J16" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="K16" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="L16" s="35"/>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
     </row>
-    <row r="17" spans="1:14" s="10" customFormat="1" ht="55.2" customHeight="1">
+    <row r="17" spans="1:14" s="10" customFormat="1" ht="55.15" customHeight="1">
       <c r="A17" s="6"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="40"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="39"/>
       <c r="D17" s="24">
         <v>3</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F17" s="24">
         <v>3</v>
       </c>
-      <c r="G17" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="J17" s="29"/>
-      <c r="K17" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="L17" s="31"/>
+      <c r="G17" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I17" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="J17" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="K17" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="L17" s="78" t="s">
+        <v>74</v>
+      </c>
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
     </row>
-    <row r="18" spans="1:14" s="10" customFormat="1" ht="67.2" customHeight="1">
+    <row r="18" spans="1:14" s="10" customFormat="1" ht="67.150000000000006" customHeight="1">
       <c r="A18" s="6"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="40"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="39"/>
       <c r="D18" s="24">
         <v>4</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F18" s="24">
         <v>4</v>
       </c>
       <c r="G18" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I18" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="J18" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="K18" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="J18" s="29"/>
-      <c r="K18" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="L18" s="31"/>
+      <c r="L18" s="77"/>
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
     </row>
-    <row r="19" spans="1:14" s="10" customFormat="1" ht="76.8" customHeight="1">
+    <row r="19" spans="1:14" s="10" customFormat="1" ht="76.900000000000006" customHeight="1">
       <c r="A19" s="6"/>
       <c r="B19" s="22">
         <v>1</v>
@@ -6154,102 +6649,102 @@
         <v>1</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F19" s="24">
         <v>1</v>
       </c>
-      <c r="G19" s="34" t="s">
+      <c r="G19" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="J19" s="34"/>
+      <c r="K19" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="J19" s="35"/>
-      <c r="K19" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="L19" s="36"/>
+      <c r="L19" s="35"/>
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
     </row>
     <row r="20" spans="1:14" ht="60.6" customHeight="1">
-      <c r="B20" s="32"/>
-      <c r="C20" s="41" t="s">
-        <v>42</v>
+      <c r="B20" s="31"/>
+      <c r="C20" s="40" t="s">
+        <v>40</v>
       </c>
       <c r="D20" s="24">
         <v>2</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F20" s="24">
         <v>2</v>
       </c>
-      <c r="G20" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="J20" s="29"/>
-      <c r="K20" s="30" t="s">
+      <c r="G20" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="L20" s="31"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="L20" s="30"/>
     </row>
     <row r="21" spans="1:14" ht="66" customHeight="1">
-      <c r="B21" s="32"/>
-      <c r="C21" s="40"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="39"/>
       <c r="D21" s="24">
         <v>3</v>
       </c>
-      <c r="E21" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="F21" s="43">
+      <c r="E21" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="42">
         <v>3</v>
       </c>
-      <c r="G21" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="J21" s="29"/>
-      <c r="K21" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="L21" s="31"/>
+      <c r="G21" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="J21" s="28"/>
+      <c r="K21" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="L21" s="30"/>
     </row>
-    <row r="22" spans="1:14" ht="55.2" customHeight="1" thickBot="1">
-      <c r="B22" s="45"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="46">
+    <row r="22" spans="1:14" ht="55.15" customHeight="1" thickBot="1">
+      <c r="B22" s="44"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="45">
         <v>4</v>
       </c>
-      <c r="E22" s="47" t="s">
-        <v>60</v>
+      <c r="E22" s="46" t="s">
+        <v>58</v>
       </c>
       <c r="F22" s="24">
         <v>4</v>
       </c>
-      <c r="G22" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="J22" s="29"/>
-      <c r="K22" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="L22" s="31"/>
+      <c r="G22" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="J22" s="28"/>
+      <c r="K22" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="L22" s="30"/>
     </row>
     <row r="23" spans="1:14" ht="51" customHeight="1">
       <c r="B23" s="22">
@@ -6260,152 +6755,152 @@
         <v>1</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F23" s="24">
         <v>1</v>
       </c>
-      <c r="G23" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="J23" s="35"/>
-      <c r="K23" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="L23" s="36"/>
+      <c r="G23" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="J23" s="34"/>
+      <c r="K23" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="L23" s="35"/>
     </row>
-    <row r="24" spans="1:14" ht="64.2" customHeight="1">
-      <c r="B24" s="32"/>
-      <c r="C24" s="38" t="s">
-        <v>52</v>
+    <row r="24" spans="1:14" ht="64.150000000000006" customHeight="1">
+      <c r="B24" s="31"/>
+      <c r="C24" s="37" t="s">
+        <v>50</v>
       </c>
       <c r="D24" s="24">
         <v>2</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F24" s="24">
         <v>2</v>
       </c>
-      <c r="G24" s="34" t="s">
+      <c r="G24" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="J24" s="28"/>
+      <c r="K24" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="J24" s="29"/>
-      <c r="K24" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="L24" s="31"/>
+      <c r="L24" s="30"/>
     </row>
-    <row r="25" spans="1:14" ht="67.8" customHeight="1">
-      <c r="B25" s="32"/>
-      <c r="C25" s="40"/>
+    <row r="25" spans="1:14" ht="67.900000000000006" customHeight="1">
+      <c r="B25" s="31"/>
+      <c r="C25" s="39"/>
       <c r="D25" s="24">
         <v>3</v>
       </c>
-      <c r="E25" s="42" t="s">
+      <c r="E25" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="42">
+        <v>3</v>
+      </c>
+      <c r="G25" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="J25" s="28"/>
+      <c r="K25" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="L25" s="30"/>
+    </row>
+    <row r="26" spans="1:14" ht="73.900000000000006" customHeight="1">
+      <c r="B26" s="31"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="48">
+        <v>4</v>
+      </c>
+      <c r="E26" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="42">
+        <v>4</v>
+      </c>
+      <c r="G26" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="H26" s="51"/>
+      <c r="I26" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="J26" s="52"/>
+      <c r="K26" s="53" t="s">
+        <v>53</v>
+      </c>
+      <c r="L26" s="54"/>
+    </row>
+    <row r="27" spans="1:14" ht="61.15" customHeight="1">
+      <c r="B27" s="55"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="57">
+        <v>5</v>
+      </c>
+      <c r="E27" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="F25" s="43">
-        <v>3</v>
-      </c>
-      <c r="G25" s="44" t="s">
+      <c r="F27" s="59">
+        <v>5</v>
+      </c>
+      <c r="G27" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28" t="s">
+      <c r="H27" s="60"/>
+      <c r="I27" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="J25" s="29"/>
-      <c r="K25" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="L25" s="31"/>
+      <c r="J27" s="61"/>
+      <c r="K27" s="62" t="s">
+        <v>53</v>
+      </c>
+      <c r="L27" s="63"/>
     </row>
-    <row r="26" spans="1:14" ht="73.8" customHeight="1">
-      <c r="B26" s="32"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="49">
-        <v>4</v>
-      </c>
-      <c r="E26" s="50" t="s">
-        <v>64</v>
-      </c>
-      <c r="F26" s="43">
-        <v>4</v>
-      </c>
-      <c r="G26" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H26" s="52"/>
-      <c r="I26" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="J26" s="53"/>
-      <c r="K26" s="54" t="s">
-        <v>55</v>
-      </c>
-      <c r="L26" s="55"/>
-    </row>
-    <row r="27" spans="1:14" ht="61.2" customHeight="1">
-      <c r="B27" s="56"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="58">
-        <v>5</v>
-      </c>
-      <c r="E27" s="59" t="s">
-        <v>65</v>
-      </c>
-      <c r="F27" s="60">
-        <v>5</v>
-      </c>
-      <c r="G27" s="66" t="s">
-        <v>56</v>
-      </c>
-      <c r="H27" s="61"/>
-      <c r="I27" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="J27" s="62"/>
-      <c r="K27" s="63" t="s">
-        <v>55</v>
-      </c>
-      <c r="L27" s="64"/>
-    </row>
-    <row r="28" spans="1:14" ht="15.6">
+    <row r="28" spans="1:14" ht="15.75">
       <c r="B28" s="12"/>
       <c r="C28" s="13"/>
     </row>
-    <row r="29" spans="1:14" ht="15.6">
+    <row r="29" spans="1:14" ht="15.75">
       <c r="B29" s="12"/>
       <c r="C29" s="13"/>
       <c r="H29" s="12"/>
     </row>
-    <row r="30" spans="1:14" ht="15.6">
+    <row r="30" spans="1:14" ht="15.75">
       <c r="B30" s="12"/>
       <c r="C30" s="13"/>
     </row>
-    <row r="31" spans="1:14" ht="15.6">
+    <row r="31" spans="1:14" ht="15.75">
       <c r="B31" s="12"/>
       <c r="C31" s="13"/>
     </row>
-    <row r="32" spans="1:14" ht="15.6">
+    <row r="32" spans="1:14" ht="15.75">
       <c r="B32" s="12"/>
       <c r="C32" s="13"/>
     </row>
-    <row r="33" spans="2:11" ht="15.6">
+    <row r="33" spans="2:11" ht="15.75">
       <c r="B33" s="12"/>
       <c r="C33" s="13"/>
     </row>
-    <row r="34" spans="2:11" ht="15.6">
+    <row r="34" spans="2:11" ht="15.75">
       <c r="B34" s="12"/>
       <c r="C34" s="13"/>
     </row>
@@ -6586,8 +7081,8 @@
     <row r="72" ht="36" customHeight="1"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{D6408F3F-69A9-4377-B307-B0A0F5ECDF86}">
-      <selection activeCell="J3" sqref="J3"/>
+    <customSheetView guid="{C61E42EC-A28A-4F34-B1F0-5B0C369C3BFF}" scale="70">
+      <selection activeCell="W13" sqref="W13"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -6596,8 +7091,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{C61E42EC-A28A-4F34-B1F0-5B0C369C3BFF}" scale="70">
-      <selection activeCell="W13" sqref="W13"/>
+    <customSheetView guid="{D6408F3F-69A9-4377-B307-B0A0F5ECDF86}">
+      <selection activeCell="J3" sqref="J3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
@@ -6612,238 +7107,398 @@
     <mergeCell ref="J10:J11"/>
   </mergeCells>
   <conditionalFormatting sqref="H12">
-    <cfRule type="containsText" dxfId="87" priority="303" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="135" priority="351" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",H12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="304" operator="containsText" text="NG">
+    <cfRule type="containsText" dxfId="134" priority="352" operator="containsText" text="NG">
       <formula>NOT(ISERROR(SEARCH("NG",H12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="cellIs" dxfId="85" priority="301" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="349" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="302" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="350" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="cellIs" dxfId="83" priority="300" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="348" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="cellIs" dxfId="82" priority="297" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="345" operator="equal">
       <formula>"OK with reason"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="298" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="346" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="299" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="347" operator="equal">
       <formula>"""OK with reason"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="containsText" dxfId="79" priority="295" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="127" priority="343" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",I12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="296" operator="containsText" text="NG">
+    <cfRule type="containsText" dxfId="126" priority="344" operator="containsText" text="NG">
       <formula>NOT(ISERROR(SEARCH("NG",I12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="cellIs" dxfId="77" priority="293" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="341" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="294" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="342" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="cellIs" dxfId="75" priority="292" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="340" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="cellIs" dxfId="74" priority="289" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="337" operator="equal">
       <formula>"OK with reason"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="290" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="338" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="291" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="339" operator="equal">
       <formula>"""OK with reason"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H14:I14">
-    <cfRule type="containsText" dxfId="71" priority="175" operator="containsText" text="OK">
-      <formula>NOT(ISERROR(SEARCH("OK",H14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="176" operator="containsText" text="NG">
-      <formula>NOT(ISERROR(SEARCH("NG",H14)))</formula>
+  <conditionalFormatting sqref="I14">
+    <cfRule type="containsText" dxfId="119" priority="223" operator="containsText" text="OK">
+      <formula>NOT(ISERROR(SEARCH("OK",I14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="118" priority="224" operator="containsText" text="NG">
+      <formula>NOT(ISERROR(SEARCH("NG",I14)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H14:I14">
-    <cfRule type="cellIs" dxfId="69" priority="173" operator="equal">
+  <conditionalFormatting sqref="I14">
+    <cfRule type="cellIs" dxfId="117" priority="221" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="174" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="222" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H14:I14">
-    <cfRule type="cellIs" dxfId="67" priority="172" operator="equal">
+  <conditionalFormatting sqref="I14">
+    <cfRule type="cellIs" dxfId="115" priority="220" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H14:I14">
-    <cfRule type="cellIs" dxfId="66" priority="169" operator="equal">
+  <conditionalFormatting sqref="I14">
+    <cfRule type="cellIs" dxfId="114" priority="217" operator="equal">
       <formula>"OK with reason"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="170" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="218" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="219" operator="equal">
+      <formula>"""OK with reason"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="containsText" dxfId="103" priority="231" operator="containsText" text="OK">
+      <formula>NOT(ISERROR(SEARCH("OK",I13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="102" priority="232" operator="containsText" text="NG">
+      <formula>NOT(ISERROR(SEARCH("NG",I13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="cellIs" dxfId="101" priority="229" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="100" priority="230" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="cellIs" dxfId="99" priority="228" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="cellIs" dxfId="98" priority="225" operator="equal">
+      <formula>"OK with reason"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="97" priority="226" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="96" priority="227" operator="equal">
+      <formula>"""OK with reason"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23:I23 H24:H26">
+    <cfRule type="containsText" dxfId="95" priority="143" operator="containsText" text="OK">
+      <formula>NOT(ISERROR(SEARCH("OK",H23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="94" priority="144" operator="containsText" text="NG">
+      <formula>NOT(ISERROR(SEARCH("NG",H23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23:I23 H24:H26">
+    <cfRule type="cellIs" dxfId="93" priority="141" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="92" priority="142" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23:I23 H24:H26">
+    <cfRule type="cellIs" dxfId="91" priority="140" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23:I23 H24:H26">
+    <cfRule type="cellIs" dxfId="90" priority="137" operator="equal">
+      <formula>"OK with reason"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="89" priority="138" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="139" operator="equal">
+      <formula>"""OK with reason"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19:I22 I15:I18">
+    <cfRule type="containsText" dxfId="87" priority="151" operator="containsText" text="OK">
+      <formula>NOT(ISERROR(SEARCH("OK",H15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="86" priority="152" operator="containsText" text="NG">
+      <formula>NOT(ISERROR(SEARCH("NG",H15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19:I22 I15:I18">
+    <cfRule type="cellIs" dxfId="85" priority="149" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="84" priority="150" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19:I22 I15:I18">
+    <cfRule type="cellIs" dxfId="83" priority="148" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19:I22 I15:I18">
+    <cfRule type="cellIs" dxfId="82" priority="145" operator="equal">
+      <formula>"OK with reason"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="81" priority="146" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="80" priority="147" operator="equal">
+      <formula>"""OK with reason"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27:I27">
+    <cfRule type="containsText" dxfId="79" priority="79" operator="containsText" text="OK">
+      <formula>NOT(ISERROR(SEARCH("OK",H27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="78" priority="80" operator="containsText" text="NG">
+      <formula>NOT(ISERROR(SEARCH("NG",H27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27:I27">
+    <cfRule type="cellIs" dxfId="77" priority="77" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="78" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27:I27">
+    <cfRule type="cellIs" dxfId="75" priority="76" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27:I27">
+    <cfRule type="cellIs" dxfId="74" priority="73" operator="equal">
+      <formula>"OK with reason"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="73" priority="74" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="75" operator="equal">
+      <formula>"""OK with reason"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26">
+    <cfRule type="containsText" dxfId="71" priority="71" operator="containsText" text="OK">
+      <formula>NOT(ISERROR(SEARCH("OK",I26)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="70" priority="72" operator="containsText" text="NG">
+      <formula>NOT(ISERROR(SEARCH("NG",I26)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26">
+    <cfRule type="cellIs" dxfId="69" priority="69" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="70" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26">
+    <cfRule type="cellIs" dxfId="67" priority="68" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26">
+    <cfRule type="cellIs" dxfId="66" priority="65" operator="equal">
+      <formula>"OK with reason"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="66" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="67" operator="equal">
+      <formula>"""OK with reason"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I25">
+    <cfRule type="containsText" dxfId="63" priority="63" operator="containsText" text="OK">
+      <formula>NOT(ISERROR(SEARCH("OK",I25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="62" priority="64" operator="containsText" text="NG">
+      <formula>NOT(ISERROR(SEARCH("NG",I25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I25">
+    <cfRule type="cellIs" dxfId="61" priority="61" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="62" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I25">
+    <cfRule type="cellIs" dxfId="59" priority="60" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I25">
+    <cfRule type="cellIs" dxfId="58" priority="57" operator="equal">
+      <formula>"OK with reason"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="58" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="59" operator="equal">
+      <formula>"""OK with reason"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24">
+    <cfRule type="containsText" dxfId="55" priority="55" operator="containsText" text="OK">
+      <formula>NOT(ISERROR(SEARCH("OK",I24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="54" priority="56" operator="containsText" text="NG">
+      <formula>NOT(ISERROR(SEARCH("NG",I24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24">
+    <cfRule type="cellIs" dxfId="53" priority="53" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="54" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24">
+    <cfRule type="cellIs" dxfId="51" priority="52" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24">
+    <cfRule type="cellIs" dxfId="50" priority="49" operator="equal">
+      <formula>"OK with reason"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="50" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="51" operator="equal">
       <formula>"""OK with reason"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="containsText" dxfId="63" priority="191" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="47" priority="47" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",H13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="192" operator="containsText" text="NG">
+    <cfRule type="containsText" dxfId="46" priority="48" operator="containsText" text="NG">
       <formula>NOT(ISERROR(SEARCH("NG",H13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="cellIs" dxfId="61" priority="189" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="45" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="190" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="cellIs" dxfId="59" priority="188" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="44" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="cellIs" dxfId="58" priority="185" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="41" operator="equal">
       <formula>"OK with reason"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="186" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="42" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="187" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="43" operator="equal">
       <formula>"""OK with reason"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="containsText" dxfId="55" priority="183" operator="containsText" text="OK">
-      <formula>NOT(ISERROR(SEARCH("OK",I13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="184" operator="containsText" text="NG">
-      <formula>NOT(ISERROR(SEARCH("NG",I13)))</formula>
+  <conditionalFormatting sqref="H14">
+    <cfRule type="containsText" dxfId="39" priority="39" operator="containsText" text="OK">
+      <formula>NOT(ISERROR(SEARCH("OK",H14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="40" operator="containsText" text="NG">
+      <formula>NOT(ISERROR(SEARCH("NG",H14)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="cellIs" dxfId="53" priority="181" operator="equal">
+  <conditionalFormatting sqref="H14">
+    <cfRule type="cellIs" dxfId="37" priority="37" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="182" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="38" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="cellIs" dxfId="51" priority="180" operator="equal">
+  <conditionalFormatting sqref="H14">
+    <cfRule type="cellIs" dxfId="35" priority="36" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="cellIs" dxfId="50" priority="177" operator="equal">
+  <conditionalFormatting sqref="H14">
+    <cfRule type="cellIs" dxfId="34" priority="33" operator="equal">
       <formula>"OK with reason"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="178" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="34" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="179" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="35" operator="equal">
       <formula>"""OK with reason"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H23:I23 H24:H26">
-    <cfRule type="containsText" dxfId="47" priority="95" operator="containsText" text="OK">
-      <formula>NOT(ISERROR(SEARCH("OK",H23)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="96" operator="containsText" text="NG">
-      <formula>NOT(ISERROR(SEARCH("NG",H23)))</formula>
+  <conditionalFormatting sqref="H15">
+    <cfRule type="containsText" dxfId="31" priority="31" operator="containsText" text="OK">
+      <formula>NOT(ISERROR(SEARCH("OK",H15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="32" operator="containsText" text="NG">
+      <formula>NOT(ISERROR(SEARCH("NG",H15)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H23:I23 H24:H26">
-    <cfRule type="cellIs" dxfId="45" priority="93" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="94" operator="equal">
-      <formula>"NG"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H23:I23 H24:H26">
-    <cfRule type="cellIs" dxfId="43" priority="92" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H23:I23 H24:H26">
-    <cfRule type="cellIs" dxfId="42" priority="89" operator="equal">
-      <formula>"OK with reason"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="90" operator="equal">
-      <formula>"NG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="91" operator="equal">
-      <formula>"""OK with reason"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H15:I22">
-    <cfRule type="containsText" dxfId="39" priority="103" operator="containsText" text="OK">
-      <formula>NOT(ISERROR(SEARCH("OK",H15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="104" operator="containsText" text="NG">
-      <formula>NOT(ISERROR(SEARCH("NG",H15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H15:I22">
-    <cfRule type="cellIs" dxfId="37" priority="101" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="102" operator="equal">
-      <formula>"NG"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H15:I22">
-    <cfRule type="cellIs" dxfId="35" priority="100" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H15:I22">
-    <cfRule type="cellIs" dxfId="34" priority="97" operator="equal">
-      <formula>"OK with reason"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="98" operator="equal">
-      <formula>"NG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="99" operator="equal">
-      <formula>"""OK with reason"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H27:I27">
-    <cfRule type="containsText" dxfId="31" priority="31" operator="containsText" text="OK">
-      <formula>NOT(ISERROR(SEARCH("OK",H27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="32" operator="containsText" text="NG">
-      <formula>NOT(ISERROR(SEARCH("NG",H27)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H27:I27">
+  <conditionalFormatting sqref="H15">
     <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -6851,12 +7506,12 @@
       <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H27:I27">
+  <conditionalFormatting sqref="H15">
     <cfRule type="cellIs" dxfId="27" priority="28" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H27:I27">
+  <conditionalFormatting sqref="H15">
     <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
       <formula>"OK with reason"</formula>
     </cfRule>
@@ -6867,15 +7522,15 @@
       <formula>"""OK with reason"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I26">
+  <conditionalFormatting sqref="H16">
     <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="OK">
-      <formula>NOT(ISERROR(SEARCH("OK",I26)))</formula>
+      <formula>NOT(ISERROR(SEARCH("OK",H16)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="NG">
-      <formula>NOT(ISERROR(SEARCH("NG",I26)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NG",H16)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I26">
+  <conditionalFormatting sqref="H16">
     <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -6883,12 +7538,12 @@
       <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I26">
+  <conditionalFormatting sqref="H16">
     <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I26">
+  <conditionalFormatting sqref="H16">
     <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
       <formula>"OK with reason"</formula>
     </cfRule>
@@ -6899,15 +7554,15 @@
       <formula>"""OK with reason"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I25">
+  <conditionalFormatting sqref="H17">
     <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="OK">
-      <formula>NOT(ISERROR(SEARCH("OK",I25)))</formula>
+      <formula>NOT(ISERROR(SEARCH("OK",H17)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="NG">
-      <formula>NOT(ISERROR(SEARCH("NG",I25)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NG",H17)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I25">
+  <conditionalFormatting sqref="H17">
     <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -6915,12 +7570,12 @@
       <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I25">
+  <conditionalFormatting sqref="H17">
     <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I25">
+  <conditionalFormatting sqref="H17">
     <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
       <formula>"OK with reason"</formula>
     </cfRule>
@@ -6931,15 +7586,15 @@
       <formula>"""OK with reason"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I24">
+  <conditionalFormatting sqref="H18">
     <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="OK">
-      <formula>NOT(ISERROR(SEARCH("OK",I24)))</formula>
+      <formula>NOT(ISERROR(SEARCH("OK",H18)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="NG">
-      <formula>NOT(ISERROR(SEARCH("NG",I24)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NG",H18)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I24">
+  <conditionalFormatting sqref="H18">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -6947,12 +7602,12 @@
       <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I24">
+  <conditionalFormatting sqref="H18">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I24">
+  <conditionalFormatting sqref="H18">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"OK with reason"</formula>
     </cfRule>

</xml_diff>